<commit_message>
Update PEC outputs after 5d202c051
</commit_message>
<xml_diff>
--- a/processed-data/rdata/spe/14_spatial_registration_PEC/PEC_spatial_annotations.xlsx
+++ b/processed-data/rdata/spe/14_spatial_registration_PEC/PEC_spatial_annotations.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1375" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1375" uniqueCount="154">
   <si>
     <t>data</t>
   </si>
@@ -58,7 +58,7 @@
     <t>Correlation values with manual layer annotations</t>
   </si>
   <si>
-    <t>Correlation values with k9 domains</t>
+    <t>Correlation values with k09 domains</t>
   </si>
   <si>
     <t>Correlation values with k16 domains</t>
@@ -181,16 +181,13 @@
     <t>L6</t>
   </si>
   <si>
-    <t>L2/3/4*</t>
-  </si>
-  <si>
     <t>L2*</t>
   </si>
   <si>
     <t>L5*</t>
   </si>
   <si>
-    <t>L4/5/3*</t>
+    <t>L4*</t>
   </si>
   <si>
     <t>L5/4*</t>
@@ -205,16 +202,13 @@
     <t>Sp09D01</t>
   </si>
   <si>
-    <t>Sp09D01/Sp09D06</t>
-  </si>
-  <si>
     <t>Sp09D06/Sp09D02</t>
   </si>
   <si>
     <t>Sp09D05/Sp09D03</t>
   </si>
   <si>
-    <t>Sp09D08/Sp09D05/Sp09D04</t>
+    <t>Sp09D08/Sp09D05</t>
   </si>
   <si>
     <t>Sp09D04</t>
@@ -232,19 +226,13 @@
     <t>Sp09D03*</t>
   </si>
   <si>
-    <t>Sp09D04/Sp09D07/Sp09D08*</t>
-  </si>
-  <si>
-    <t>Sp09D08/Sp09D05</t>
+    <t>Sp09D04/Sp09D07*</t>
   </si>
   <si>
     <t>Sp09D05/Sp09D08/Sp09D03/Sp09D04</t>
   </si>
   <si>
     <t>Sp09D08</t>
-  </si>
-  <si>
-    <t>Sp09D08/Sp09D04/Sp09D05</t>
   </si>
   <si>
     <t>Sp16D06/Sp16D15</t>
@@ -259,127 +247,88 @@
     <t>Sp16D06/Sp16D01/Sp16D15</t>
   </si>
   <si>
-    <t>Sp16D03/Sp16D08/Sp16D09</t>
+    <t>Sp16D03/Sp16D08</t>
   </si>
   <si>
-    <t>Sp16D09/Sp16D05/Sp16D03/Sp16D04/Sp16D16/Sp16D07</t>
+    <t>Sp16D09</t>
   </si>
   <si>
-    <t>Sp16D04/Sp16D16/Sp16D07/Sp16D12/Sp16D09/Sp16D05</t>
-  </si>
-  <si>
-    <t>Sp16D04/Sp16D16/Sp16D07/Sp16D09/Sp16D05/Sp16D12/Sp16D03</t>
-  </si>
-  <si>
-    <t>Sp16D07/Sp16D09/Sp16D03/Sp16D05/Sp16D04/Sp16D08/Sp16D16/Sp16D12/Sp16D10</t>
+    <t>Sp16D04/Sp16D16</t>
   </si>
   <si>
     <t>Sp16D07</t>
   </si>
   <si>
-    <t>Sp16D09/Sp16D03/Sp16D08/Sp16D10/Sp16D05/Sp16D16/Sp16D04</t>
+    <t>Sp16D09/Sp16D03/Sp16D08/Sp16D10/Sp16D05</t>
   </si>
   <si>
-    <t>Sp16D08/Sp16D10/Sp16D03/Sp16D09/Sp16D05/Sp16D16/Sp16D04</t>
+    <t>Sp16D08</t>
   </si>
   <si>
-    <t>Sp16D10/Sp16D08/Sp16D03/Sp16D09/Sp16D16/Sp16D05/Sp16D04*</t>
+    <t>Sp16D10/Sp16D08*</t>
   </si>
   <si>
-    <t>Sp16D08/Sp16D10/Sp16D03/Sp16D09</t>
+    <t>Sp16D04/Sp16D09/Sp16D07*</t>
   </si>
   <si>
-    <t>Sp16D04/Sp16D09/Sp16D07/Sp16D16/Sp16D05/Sp16D12/Sp16D03*</t>
+    <t>Sp16D09/Sp16D05/Sp16D03/Sp16D04</t>
+  </si>
+  <si>
+    <t>Sp16D09/Sp16D03/Sp16D16/Sp16D04/Sp16D05/Sp16D08/Sp16D10</t>
+  </si>
+  <si>
+    <t>Sp16D05/Sp16D09</t>
+  </si>
+  <si>
+    <t>Sp16D05/Sp16D09/Sp16D16</t>
+  </si>
+  <si>
+    <t>L3/5/4</t>
+  </si>
+  <si>
+    <t>Sp09D01/Sp09D06</t>
+  </si>
+  <si>
+    <t>Sp09D05</t>
+  </si>
+  <si>
+    <t>Sp09D05/Sp09D08</t>
+  </si>
+  <si>
+    <t>Sp09D05/Sp09D03/Sp09D08</t>
+  </si>
+  <si>
+    <t>Sp09D08/Sp09D05/Sp09D04/Sp09D03</t>
+  </si>
+  <si>
+    <t>Sp16D06</t>
+  </si>
+  <si>
+    <t>Sp16D14</t>
+  </si>
+  <si>
+    <t>Sp16D03/Sp16D09/Sp16D08/Sp16D05</t>
+  </si>
+  <si>
+    <t>Sp16D09/Sp16D03/Sp16D05/Sp16D07</t>
+  </si>
+  <si>
+    <t>Sp16D08/Sp16D10/Sp16D03/Sp16D16/Sp16D09/Sp16D05/Sp16D04</t>
+  </si>
+  <si>
+    <t>Sp16D08/Sp16D03/Sp16D10/Sp16D09/Sp16D05/Sp16D16</t>
   </si>
   <si>
     <t>Sp16D09/Sp16D05/Sp16D03/Sp16D04/Sp16D07/Sp16D16</t>
   </si>
   <si>
-    <t>Sp16D09/Sp16D03/Sp16D16/Sp16D04/Sp16D05/Sp16D08/Sp16D10/Sp16D07</t>
+    <t>Sp16D05/Sp16D09/Sp16D03/Sp16D16</t>
   </si>
   <si>
-    <t>Sp16D05/Sp16D09/Sp16D03/Sp16D16/Sp16D04/Sp16D08/Sp16D10</t>
+    <t>Sp16D09/Sp16D16/Sp16D05/Sp16D03/Sp16D04</t>
   </si>
   <si>
-    <t>Sp16D05/Sp16D09/Sp16D16/Sp16D03/Sp16D04</t>
-  </si>
-  <si>
-    <t>L1/WM</t>
-  </si>
-  <si>
-    <t>L3/5/4</t>
-  </si>
-  <si>
-    <t>L4*</t>
-  </si>
-  <si>
-    <t>L4/5*</t>
-  </si>
-  <si>
-    <t>Sp09D05/Sp09D03/Sp09D08</t>
-  </si>
-  <si>
-    <t>Sp09D05/Sp09D08/Sp09D04</t>
-  </si>
-  <si>
-    <t>Sp09D05/Sp09D08/Sp09D07/Sp09D03/Sp09D04</t>
-  </si>
-  <si>
-    <t>Sp09D03/Sp09D05/Sp09D08/Sp09D04*</t>
-  </si>
-  <si>
-    <t>Sp09D03/Sp09D05</t>
-  </si>
-  <si>
-    <t>Sp09D05/Sp09D08/Sp09D04/Sp09D07</t>
-  </si>
-  <si>
-    <t>Sp09D08/Sp09D05/Sp09D04/Sp09D03</t>
-  </si>
-  <si>
-    <t>Sp09D08/Sp09D05/Sp09D04/Sp09D03/Sp09D07</t>
-  </si>
-  <si>
-    <t>Sp16D06/Sp16D15/Sp16D11/Sp16D13</t>
-  </si>
-  <si>
-    <t>Sp16D06/Sp16D15/Sp16D01/Sp16D11/Sp16D14</t>
-  </si>
-  <si>
-    <t>Sp16D04/Sp16D16/Sp16D09/Sp16D07/Sp16D05/Sp16D12/Sp16D03</t>
-  </si>
-  <si>
-    <t>Sp16D03/Sp16D09/Sp16D08/Sp16D05</t>
-  </si>
-  <si>
-    <t>Sp16D09/Sp16D05/Sp16D03/Sp16D04/Sp16D16/Sp16D07/Sp16D08/Sp16D10/Sp16D12</t>
-  </si>
-  <si>
-    <t>Sp16D09/Sp16D03/Sp16D05/Sp16D07/Sp16D04/Sp16D08/Sp16D16</t>
-  </si>
-  <si>
-    <t>Sp16D03/Sp16D08/Sp16D09/Sp16D05/Sp16D16/Sp16D10</t>
-  </si>
-  <si>
-    <t>Sp16D08/Sp16D03/Sp16D09/Sp16D10/Sp16D05/Sp16D16/Sp16D04</t>
-  </si>
-  <si>
-    <t>Sp16D08/Sp16D10/Sp16D03/Sp16D16/Sp16D09/Sp16D05/Sp16D04</t>
-  </si>
-  <si>
-    <t>Sp16D08/Sp16D03/Sp16D10/Sp16D09/Sp16D05/Sp16D16/Sp16D04</t>
-  </si>
-  <si>
-    <t>Sp16D09/Sp16D16/Sp16D05/Sp16D03/Sp16D04/Sp16D08/Sp16D10/Sp16D07</t>
-  </si>
-  <si>
-    <t>Sp16D09/Sp16D16/Sp16D04/Sp16D05/Sp16D03/Sp16D08/Sp16D07/Sp16D10</t>
-  </si>
-  <si>
-    <t>WM/L1</t>
-  </si>
-  <si>
-    <t>L3/6</t>
+    <t>Sp16D09/Sp16D16/Sp16D04/Sp16D05/Sp16D03/Sp16D08</t>
   </si>
   <si>
     <t>Sp09D08*</t>
@@ -388,25 +337,13 @@
     <t>Sp09D02*</t>
   </si>
   <si>
-    <t>Sp09D05/Sp09D08/Sp09D04/Sp09D07/Sp09D03</t>
+    <t>Sp09D07/Sp09D05</t>
   </si>
   <si>
-    <t>Sp09D04/Sp09D08/Sp09D05/Sp09D07</t>
+    <t>Sp16D03</t>
   </si>
   <si>
-    <t>Sp09D07/Sp09D05/Sp09D08</t>
-  </si>
-  <si>
-    <t>Sp16D06/Sp16D01/Sp16D15/Sp16D14/Sp16D11</t>
-  </si>
-  <si>
-    <t>Sp16D03/Sp16D08/Sp16D09/Sp16D05/Sp16D10/Sp16D07</t>
-  </si>
-  <si>
-    <t>Sp16D09/Sp16D08/Sp16D05/Sp16D16/Sp16D03/Sp16D04*</t>
-  </si>
-  <si>
-    <t>Sp16D08</t>
+    <t>Sp16D09/Sp16D08/Sp16D05/Sp16D16/Sp16D03*</t>
   </si>
   <si>
     <t>Sp16D08*</t>
@@ -415,28 +352,25 @@
     <t>Sp16D02*</t>
   </si>
   <si>
-    <t>Sp16D05/Sp16D09/Sp16D16/Sp16D04/Sp16D03</t>
+    <t>Sp16D04</t>
   </si>
   <si>
-    <t>Sp16D05/Sp16D16/Sp16D09/Sp16D04/Sp16D03/Sp16D10/Sp16D08</t>
+    <t>Sp16D05/Sp16D09/Sp16D16/Sp16D04</t>
   </si>
   <si>
-    <t>Sp16D09/Sp16D05/Sp16D03/Sp16D04/Sp16D07/Sp16D16/Sp16D08/Sp16D10</t>
+    <t>Sp16D05/Sp16D16/Sp16D09</t>
   </si>
   <si>
-    <t>Sp16D09/Sp16D16/Sp16D04/Sp16D05/Sp16D03/Sp16D08/Sp16D10/Sp16D07</t>
+    <t>Sp16D04/Sp16D16/Sp16D09/Sp16D05/Sp16D07</t>
   </si>
   <si>
-    <t>Sp16D09/Sp16D04/Sp16D05/Sp16D03/Sp16D16/Sp16D07</t>
+    <t>Sp16D07/Sp16D09/Sp16D03/Sp16D05</t>
   </si>
   <si>
-    <t>Sp16D04/Sp16D16/Sp16D09/Sp16D05/Sp16D07/Sp16D03/Sp16D12</t>
+    <t>L4/5*</t>
   </si>
   <si>
-    <t>Sp16D07/Sp16D09/Sp16D03/Sp16D05/Sp16D04/Sp16D08/Sp16D16/Sp16D10/Sp16D12</t>
-  </si>
-  <si>
-    <t>L6/5*</t>
+    <t>L6*</t>
   </si>
   <si>
     <t>L2/4/3*</t>
@@ -445,58 +379,31 @@
     <t>Sp09D06/Sp09D01</t>
   </si>
   <si>
-    <t>Sp09D06/Sp09D02/Sp09D09</t>
+    <t>Sp09D07/Sp09D08*</t>
   </si>
   <si>
-    <t>Sp09D04/Sp09D07</t>
+    <t>Sp09D08/Sp09D05/Sp09D03*</t>
   </si>
   <si>
-    <t>Sp09D05</t>
+    <t>Sp16D16/Sp16D04</t>
   </si>
   <si>
-    <t>Sp09D05/Sp09D07/Sp09D08/Sp09D03/Sp09D04</t>
+    <t>Sp16D03/Sp16D09</t>
   </si>
   <si>
-    <t>Sp09D07/Sp09D08/Sp09D05/Sp09D04*</t>
+    <t>Sp16D03/Sp16D09/Sp16D07/Sp16D05</t>
   </si>
   <si>
-    <t>Sp09D08/Sp09D05/Sp09D03/Sp09D04*</t>
+    <t>Sp16D09/Sp16D16/Sp16D05/Sp16D03/Sp16D08/Sp16D04</t>
   </si>
   <si>
-    <t>Sp16D06/Sp16D15/Sp16D01/Sp16D11/Sp16D14/Sp16D13</t>
-  </si>
-  <si>
-    <t>Sp16D03/Sp16D08</t>
-  </si>
-  <si>
-    <t>Sp16D04/Sp16D07/Sp16D16/Sp16D09/Sp16D12/Sp16D05/Sp16D03</t>
-  </si>
-  <si>
-    <t>Sp16D16/Sp16D04/Sp16D09/Sp16D07/Sp16D05/Sp16D03/Sp16D12</t>
-  </si>
-  <si>
-    <t>Sp16D09/Sp16D05/Sp16D04/Sp16D03/Sp16D16/Sp16D07</t>
-  </si>
-  <si>
-    <t>Sp16D03/Sp16D09/Sp16D05/Sp16D04/Sp16D07/Sp16D08/Sp16D16/Sp16D10</t>
-  </si>
-  <si>
-    <t>Sp16D03/Sp16D09/Sp16D07/Sp16D05/Sp16D08/Sp16D16/Sp16D04/Sp16D12/Sp16D10</t>
-  </si>
-  <si>
-    <t>Sp16D09/Sp16D16/Sp16D05/Sp16D03/Sp16D08/Sp16D04/Sp16D10/Sp16D07</t>
+    <t>Sp16D05/Sp16D09/Sp16D16/Sp16D04/Sp16D03</t>
   </si>
   <si>
     <t>Sp16D09/Sp16D16/Sp16D05/Sp16D07/Sp16D04/Sp16D12/Sp16D03*</t>
   </si>
   <si>
-    <t>Sp16D09/Sp16D08/Sp16D05/Sp16D03/Sp16D10/Sp16D16/Sp16D04</t>
-  </si>
-  <si>
-    <t>Sp16D08/Sp16D10/Sp16D09/Sp16D03/Sp16D16/Sp16D05/Sp16D04*</t>
-  </si>
-  <si>
-    <t>L4/3/5/2*</t>
+    <t>Sp16D08/Sp16D10*</t>
   </si>
   <si>
     <t>L4/3/5</t>
@@ -505,22 +412,10 @@
     <t>L4/2/3*</t>
   </si>
   <si>
-    <t>Sp09D08/Sp09D05/Sp09D04/Sp09D07</t>
+    <t>L3/6</t>
   </si>
   <si>
-    <t>Sp09D07/Sp09D05/Sp09D08/Sp09D03/Sp09D04</t>
-  </si>
-  <si>
-    <t>Sp16D09/Sp16D05/Sp16D16/Sp16D03/Sp16D04/Sp16D08</t>
-  </si>
-  <si>
-    <t>Sp16D09/Sp16D05/Sp16D03/Sp16D08/Sp16D16/Sp16D04</t>
-  </si>
-  <si>
-    <t>Sp16D08/Sp16D09/Sp16D10/Sp16D04/Sp16D16/Sp16D03/Sp16D05*</t>
-  </si>
-  <si>
-    <t>Sp16D07/Sp16D09/Sp16D03/Sp16D05/Sp16D08/Sp16D04/Sp16D16/Sp16D12/Sp16D10</t>
+    <t>Sp09D08/Sp09D05*</t>
   </si>
   <si>
     <t>Micro.PVM</t>
@@ -580,19 +475,7 @@
     <t>Sp16D02</t>
   </si>
   <si>
-    <t>Sp16D03</t>
-  </si>
-  <si>
-    <t>Sp16D04</t>
-  </si>
-  <si>
     <t>Sp16D05</t>
-  </si>
-  <si>
-    <t>Sp16D06</t>
-  </si>
-  <si>
-    <t>Sp16D09</t>
   </si>
   <si>
     <t>Sp16D10</t>
@@ -605,9 +488,6 @@
   </si>
   <si>
     <t>Sp16D13</t>
-  </si>
-  <si>
-    <t>Sp16D14</t>
   </si>
   <si>
     <t>Sp16D15</t>
@@ -723,7 +603,7 @@
         <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>163</v>
+        <v>128</v>
       </c>
       <c r="D1" t="s">
         <v>22</v>
@@ -738,28 +618,28 @@
         <v>20</v>
       </c>
       <c r="H1" t="s">
-        <v>169</v>
+        <v>134</v>
       </c>
       <c r="I1" t="s">
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="J1" t="s">
         <v>30</v>
       </c>
       <c r="K1" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
       <c r="L1" t="s">
-        <v>167</v>
+        <v>132</v>
       </c>
       <c r="M1" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="N1" t="s">
-        <v>165</v>
+        <v>130</v>
       </c>
       <c r="O1" t="s">
-        <v>168</v>
+        <v>133</v>
       </c>
       <c r="P1" t="s">
         <v>34</v>
@@ -774,7 +654,7 @@
         <v>35</v>
       </c>
       <c r="T1" t="s">
-        <v>173</v>
+        <v>138</v>
       </c>
       <c r="U1" t="s">
         <v>39</v>
@@ -783,7 +663,7 @@
         <v>40</v>
       </c>
       <c r="W1" t="s">
-        <v>171</v>
+        <v>136</v>
       </c>
       <c r="X1" t="s">
         <v>38</v>
@@ -865,7 +745,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>174</v>
+        <v>139</v>
       </c>
       <c r="B3" t="n">
         <v>-0.03454803270631968</v>
@@ -939,7 +819,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>175</v>
+        <v>140</v>
       </c>
       <c r="B4" t="n">
         <v>-0.27108358554851375</v>
@@ -1013,7 +893,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>176</v>
+        <v>141</v>
       </c>
       <c r="B5" t="n">
         <v>-0.27948716671215584</v>
@@ -1087,7 +967,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>177</v>
+        <v>142</v>
       </c>
       <c r="B6" t="n">
         <v>-0.4071713807333885</v>
@@ -1161,7 +1041,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>178</v>
+        <v>143</v>
       </c>
       <c r="B7" t="n">
         <v>-0.3189287446211929</v>
@@ -1235,7 +1115,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>179</v>
+        <v>144</v>
       </c>
       <c r="B8" t="n">
         <v>0.021729604641251715</v>
@@ -1338,7 +1218,7 @@
         <v>38</v>
       </c>
       <c r="G1" t="s">
-        <v>171</v>
+        <v>136</v>
       </c>
       <c r="H1" t="s">
         <v>39</v>
@@ -1347,31 +1227,31 @@
         <v>40</v>
       </c>
       <c r="J1" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
       <c r="K1" t="s">
-        <v>167</v>
+        <v>132</v>
       </c>
       <c r="L1" t="s">
-        <v>169</v>
+        <v>134</v>
       </c>
       <c r="M1" t="s">
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="N1" t="s">
         <v>30</v>
       </c>
       <c r="O1" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="P1" t="s">
-        <v>168</v>
+        <v>133</v>
       </c>
       <c r="Q1" t="s">
-        <v>165</v>
+        <v>130</v>
       </c>
       <c r="R1" t="s">
-        <v>173</v>
+        <v>138</v>
       </c>
       <c r="S1" t="s">
         <v>17</v>
@@ -1386,7 +1266,7 @@
         <v>18</v>
       </c>
       <c r="W1" t="s">
-        <v>163</v>
+        <v>128</v>
       </c>
       <c r="X1" t="s">
         <v>22</v>
@@ -1394,7 +1274,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" t="n">
         <v>-0.19642471190308702</v>
@@ -1468,7 +1348,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" t="n">
         <v>0.05241809113899626</v>
@@ -1542,7 +1422,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B4" t="n">
         <v>0.26271496353564744</v>
@@ -1616,7 +1496,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B5" t="n">
         <v>0.08712895801930914</v>
@@ -1690,7 +1570,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>139</v>
+        <v>85</v>
       </c>
       <c r="B6" t="n">
         <v>0.18331765182362297</v>
@@ -1764,7 +1644,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7" t="n">
         <v>-0.1467381610821228</v>
@@ -1838,7 +1718,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B8" t="n">
         <v>-0.005920366538321899</v>
@@ -1912,7 +1792,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B9" t="n">
         <v>0.15089624526754253</v>
@@ -1986,7 +1866,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>180</v>
+        <v>145</v>
       </c>
       <c r="B10" t="n">
         <v>-0.1809097158651717</v>
@@ -2089,7 +1969,7 @@
         <v>39</v>
       </c>
       <c r="G1" t="s">
-        <v>171</v>
+        <v>136</v>
       </c>
       <c r="H1" t="s">
         <v>40</v>
@@ -2098,31 +1978,31 @@
         <v>38</v>
       </c>
       <c r="J1" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
       <c r="K1" t="s">
-        <v>167</v>
+        <v>132</v>
       </c>
       <c r="L1" t="s">
-        <v>169</v>
+        <v>134</v>
       </c>
       <c r="M1" t="s">
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="N1" t="s">
         <v>30</v>
       </c>
       <c r="O1" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="P1" t="s">
-        <v>168</v>
+        <v>133</v>
       </c>
       <c r="Q1" t="s">
-        <v>165</v>
+        <v>130</v>
       </c>
       <c r="R1" t="s">
-        <v>173</v>
+        <v>138</v>
       </c>
       <c r="S1" t="s">
         <v>17</v>
@@ -2137,7 +2017,7 @@
         <v>18</v>
       </c>
       <c r="W1" t="s">
-        <v>163</v>
+        <v>128</v>
       </c>
       <c r="X1" t="s">
         <v>22</v>
@@ -2145,7 +2025,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B2" t="n">
         <v>-0.21673408049258922</v>
@@ -2219,7 +2099,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>181</v>
+        <v>146</v>
       </c>
       <c r="B3" t="n">
         <v>0.06796189545137604</v>
@@ -2293,7 +2173,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>182</v>
+        <v>102</v>
       </c>
       <c r="B4" t="n">
         <v>0.24855420334162878</v>
@@ -2367,7 +2247,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>183</v>
+        <v>106</v>
       </c>
       <c r="B5" t="n">
         <v>0.16239924004104697</v>
@@ -2441,7 +2321,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>184</v>
+        <v>147</v>
       </c>
       <c r="B6" t="n">
         <v>0.21673710260742649</v>
@@ -2515,7 +2395,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>185</v>
+        <v>89</v>
       </c>
       <c r="B7" t="n">
         <v>-0.2361586152281981</v>
@@ -2589,7 +2469,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B8" t="n">
         <v>0.0648001484142263</v>
@@ -2663,7 +2543,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>124</v>
+        <v>76</v>
       </c>
       <c r="B9" t="n">
         <v>0.28730991325806404</v>
@@ -2737,7 +2617,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>186</v>
+        <v>72</v>
       </c>
       <c r="B10" t="n">
         <v>0.23589202470987386</v>
@@ -2811,7 +2691,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>187</v>
+        <v>148</v>
       </c>
       <c r="B11" t="n">
         <v>0.22713757882093236</v>
@@ -2885,7 +2765,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>188</v>
+        <v>149</v>
       </c>
       <c r="B12" t="n">
         <v>-0.22278141482988542</v>
@@ -2959,7 +2839,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>189</v>
+        <v>150</v>
       </c>
       <c r="B13" t="n">
         <v>0.022087253506472327</v>
@@ -3033,7 +2913,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>190</v>
+        <v>151</v>
       </c>
       <c r="B14" t="n">
         <v>-0.22458840453467374</v>
@@ -3107,7 +2987,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>191</v>
+        <v>90</v>
       </c>
       <c r="B15" t="n">
         <v>-0.07795973364557778</v>
@@ -3181,7 +3061,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>192</v>
+        <v>152</v>
       </c>
       <c r="B16" t="n">
         <v>-0.23417046391770813</v>
@@ -3255,7 +3135,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>193</v>
+        <v>153</v>
       </c>
       <c r="B17" t="n">
         <v>0.2016892789220219</v>
@@ -3358,13 +3238,13 @@
         <v>19</v>
       </c>
       <c r="G1" t="s">
-        <v>163</v>
+        <v>128</v>
       </c>
       <c r="H1" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="I1" t="s">
-        <v>171</v>
+        <v>136</v>
       </c>
       <c r="J1" t="s">
         <v>35</v>
@@ -3379,7 +3259,7 @@
         <v>34</v>
       </c>
       <c r="N1" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
       <c r="O1" t="s">
         <v>39</v>
@@ -3388,25 +3268,25 @@
         <v>40</v>
       </c>
       <c r="Q1" t="s">
-        <v>173</v>
+        <v>138</v>
       </c>
       <c r="R1" t="s">
         <v>38</v>
       </c>
       <c r="S1" t="s">
-        <v>165</v>
+        <v>130</v>
       </c>
       <c r="T1" t="s">
-        <v>167</v>
+        <v>132</v>
       </c>
       <c r="U1" t="s">
-        <v>168</v>
+        <v>133</v>
       </c>
       <c r="V1" t="s">
-        <v>169</v>
+        <v>134</v>
       </c>
       <c r="W1" t="s">
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="X1" t="s">
         <v>30</v>
@@ -3488,7 +3368,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>174</v>
+        <v>139</v>
       </c>
       <c r="B3" t="n">
         <v>-0.055656183853921806</v>
@@ -3562,7 +3442,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>175</v>
+        <v>140</v>
       </c>
       <c r="B4" t="n">
         <v>-0.2780320830046695</v>
@@ -3636,7 +3516,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>176</v>
+        <v>141</v>
       </c>
       <c r="B5" t="n">
         <v>-0.2570396119823288</v>
@@ -3710,7 +3590,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>177</v>
+        <v>142</v>
       </c>
       <c r="B6" t="n">
         <v>-0.36620975240587694</v>
@@ -3784,7 +3664,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>178</v>
+        <v>143</v>
       </c>
       <c r="B7" t="n">
         <v>-0.29315224207222135</v>
@@ -3858,7 +3738,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>179</v>
+        <v>144</v>
       </c>
       <c r="B8" t="n">
         <v>0.03291208419963695</v>
@@ -3955,7 +3835,7 @@
         <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>163</v>
+        <v>128</v>
       </c>
       <c r="F1" t="s">
         <v>18</v>
@@ -3973,25 +3853,25 @@
         <v>32</v>
       </c>
       <c r="K1" t="s">
-        <v>171</v>
+        <v>136</v>
       </c>
       <c r="L1" t="s">
         <v>35</v>
       </c>
       <c r="M1" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
       <c r="N1" t="s">
-        <v>169</v>
+        <v>134</v>
       </c>
       <c r="O1" t="s">
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="P1" t="s">
         <v>30</v>
       </c>
       <c r="Q1" t="s">
-        <v>173</v>
+        <v>138</v>
       </c>
       <c r="R1" t="s">
         <v>38</v>
@@ -4003,21 +3883,21 @@
         <v>40</v>
       </c>
       <c r="U1" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="V1" t="s">
-        <v>167</v>
+        <v>132</v>
       </c>
       <c r="W1" t="s">
-        <v>165</v>
+        <v>130</v>
       </c>
       <c r="X1" t="s">
-        <v>168</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" t="n">
         <v>0.07657005433999246</v>
@@ -4091,7 +3971,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" t="n">
         <v>0.1389426928127189</v>
@@ -4165,7 +4045,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B4" t="n">
         <v>-0.5160270556350461</v>
@@ -4239,7 +4119,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B5" t="n">
         <v>-0.401109079704267</v>
@@ -4313,7 +4193,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>139</v>
+        <v>85</v>
       </c>
       <c r="B6" t="n">
         <v>-0.6048791826442408</v>
@@ -4387,7 +4267,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7" t="n">
         <v>0.8406617494978089</v>
@@ -4461,7 +4341,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B8" t="n">
         <v>-0.3143971691095612</v>
@@ -4535,7 +4415,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B9" t="n">
         <v>-0.46528915036352375</v>
@@ -4609,7 +4489,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>180</v>
+        <v>145</v>
       </c>
       <c r="B10" t="n">
         <v>0.6221965469462859</v>
@@ -4709,7 +4589,7 @@
         <v>18</v>
       </c>
       <c r="F1" t="s">
-        <v>163</v>
+        <v>128</v>
       </c>
       <c r="G1" t="s">
         <v>22</v>
@@ -4718,7 +4598,7 @@
         <v>33</v>
       </c>
       <c r="I1" t="s">
-        <v>171</v>
+        <v>136</v>
       </c>
       <c r="J1" t="s">
         <v>32</v>
@@ -4730,19 +4610,19 @@
         <v>35</v>
       </c>
       <c r="M1" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
       <c r="N1" t="s">
-        <v>169</v>
+        <v>134</v>
       </c>
       <c r="O1" t="s">
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="P1" t="s">
         <v>30</v>
       </c>
       <c r="Q1" t="s">
-        <v>173</v>
+        <v>138</v>
       </c>
       <c r="R1" t="s">
         <v>38</v>
@@ -4754,21 +4634,21 @@
         <v>40</v>
       </c>
       <c r="U1" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="V1" t="s">
-        <v>167</v>
+        <v>132</v>
       </c>
       <c r="W1" t="s">
-        <v>165</v>
+        <v>130</v>
       </c>
       <c r="X1" t="s">
-        <v>168</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B2" t="n">
         <v>0.05320113646624479</v>
@@ -4842,7 +4722,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>181</v>
+        <v>146</v>
       </c>
       <c r="B3" t="n">
         <v>-0.020433459925351123</v>
@@ -4916,7 +4796,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>182</v>
+        <v>102</v>
       </c>
       <c r="B4" t="n">
         <v>-0.6529850628776628</v>
@@ -4990,7 +4870,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>183</v>
+        <v>106</v>
       </c>
       <c r="B5" t="n">
         <v>-0.4608367336806875</v>
@@ -5064,7 +4944,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>184</v>
+        <v>147</v>
       </c>
       <c r="B6" t="n">
         <v>-0.5230867412191542</v>
@@ -5138,7 +5018,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>185</v>
+        <v>89</v>
       </c>
       <c r="B7" t="n">
         <v>0.8409048832178526</v>
@@ -5212,7 +5092,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B8" t="n">
         <v>-0.40770933184510455</v>
@@ -5286,7 +5166,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>124</v>
+        <v>76</v>
       </c>
       <c r="B9" t="n">
         <v>-0.5808168134042269</v>
@@ -5360,7 +5240,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>186</v>
+        <v>72</v>
       </c>
       <c r="B10" t="n">
         <v>-0.5774870187570127</v>
@@ -5434,7 +5314,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>187</v>
+        <v>148</v>
       </c>
       <c r="B11" t="n">
         <v>-0.4901993628333988</v>
@@ -5508,7 +5388,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>188</v>
+        <v>149</v>
       </c>
       <c r="B12" t="n">
         <v>0.6229997872894321</v>
@@ -5582,7 +5462,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>189</v>
+        <v>150</v>
       </c>
       <c r="B13" t="n">
         <v>-0.20985159820694804</v>
@@ -5656,7 +5536,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>190</v>
+        <v>151</v>
       </c>
       <c r="B14" t="n">
         <v>0.572543266319401</v>
@@ -5730,7 +5610,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>191</v>
+        <v>90</v>
       </c>
       <c r="B15" t="n">
         <v>0.14465157461277112</v>
@@ -5804,7 +5684,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>192</v>
+        <v>152</v>
       </c>
       <c r="B16" t="n">
         <v>0.7969841410084584</v>
@@ -5878,7 +5758,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>193</v>
+        <v>153</v>
       </c>
       <c r="B17" t="n">
         <v>-0.4535532435085522</v>
@@ -5978,34 +5858,34 @@
         <v>20</v>
       </c>
       <c r="F1" t="s">
-        <v>163</v>
+        <v>128</v>
       </c>
       <c r="G1" t="s">
         <v>22</v>
       </c>
       <c r="H1" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="I1" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
       <c r="J1" t="s">
-        <v>167</v>
+        <v>132</v>
       </c>
       <c r="K1" t="s">
-        <v>165</v>
+        <v>130</v>
       </c>
       <c r="L1" t="s">
-        <v>173</v>
+        <v>138</v>
       </c>
       <c r="M1" t="s">
-        <v>168</v>
+        <v>133</v>
       </c>
       <c r="N1" t="s">
-        <v>169</v>
+        <v>134</v>
       </c>
       <c r="O1" t="s">
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="P1" t="s">
         <v>30</v>
@@ -6020,10 +5900,10 @@
         <v>40</v>
       </c>
       <c r="T1" t="s">
-        <v>172</v>
+        <v>137</v>
       </c>
       <c r="U1" t="s">
-        <v>171</v>
+        <v>136</v>
       </c>
       <c r="V1" t="s">
         <v>33</v>
@@ -6117,7 +5997,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>174</v>
+        <v>139</v>
       </c>
       <c r="B3" t="n">
         <v>-0.07152760004684637</v>
@@ -6194,7 +6074,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>175</v>
+        <v>140</v>
       </c>
       <c r="B4" t="n">
         <v>-0.2670301063609448</v>
@@ -6271,7 +6151,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>176</v>
+        <v>141</v>
       </c>
       <c r="B5" t="n">
         <v>-0.22593305129520752</v>
@@ -6348,7 +6228,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>177</v>
+        <v>142</v>
       </c>
       <c r="B6" t="n">
         <v>-0.3544529003150845</v>
@@ -6425,7 +6305,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>178</v>
+        <v>143</v>
       </c>
       <c r="B7" t="n">
         <v>-0.31065772335814107</v>
@@ -6502,7 +6382,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>179</v>
+        <v>144</v>
       </c>
       <c r="B8" t="n">
         <v>0.031230914594695153</v>
@@ -6593,28 +6473,28 @@
     <row r="1">
       <c r="A1"/>
       <c r="B1" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
       <c r="C1" t="s">
-        <v>169</v>
+        <v>134</v>
       </c>
       <c r="D1" t="s">
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="E1" t="s">
         <v>30</v>
       </c>
       <c r="F1" t="s">
-        <v>168</v>
+        <v>133</v>
       </c>
       <c r="G1" t="s">
-        <v>165</v>
+        <v>130</v>
       </c>
       <c r="H1" t="s">
-        <v>167</v>
+        <v>132</v>
       </c>
       <c r="I1" t="s">
-        <v>173</v>
+        <v>138</v>
       </c>
       <c r="J1" t="s">
         <v>39</v>
@@ -6626,10 +6506,10 @@
         <v>38</v>
       </c>
       <c r="M1" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="N1" t="s">
-        <v>172</v>
+        <v>137</v>
       </c>
       <c r="O1" t="s">
         <v>33</v>
@@ -6641,7 +6521,7 @@
         <v>32</v>
       </c>
       <c r="R1" t="s">
-        <v>171</v>
+        <v>136</v>
       </c>
       <c r="S1" t="s">
         <v>35</v>
@@ -6659,7 +6539,7 @@
         <v>18</v>
       </c>
       <c r="X1" t="s">
-        <v>163</v>
+        <v>128</v>
       </c>
       <c r="Y1" t="s">
         <v>22</v>
@@ -6667,7 +6547,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" t="n">
         <v>-0.37907527139284114</v>
@@ -6744,7 +6624,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" t="n">
         <v>-0.38165829197553736</v>
@@ -6821,7 +6701,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B4" t="n">
         <v>0.12328653457040493</v>
@@ -6898,7 +6778,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B5" t="n">
         <v>0.554165776778059</v>
@@ -6975,7 +6855,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>139</v>
+        <v>85</v>
       </c>
       <c r="B6" t="n">
         <v>0.2832131782154116</v>
@@ -7052,7 +6932,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7" t="n">
         <v>-0.2877911559908785</v>
@@ -7129,7 +7009,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B8" t="n">
         <v>0.45299266803640326</v>
@@ -7206,7 +7086,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B9" t="n">
         <v>0.3239901052354487</v>
@@ -7283,7 +7163,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>180</v>
+        <v>145</v>
       </c>
       <c r="B10" t="n">
         <v>-0.06790297432864835</v>
@@ -7383,13 +7263,13 @@
         <v>38</v>
       </c>
       <c r="E1" t="s">
-        <v>172</v>
+        <v>137</v>
       </c>
       <c r="F1" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="G1" t="s">
-        <v>171</v>
+        <v>136</v>
       </c>
       <c r="H1" t="s">
         <v>35</v>
@@ -7404,28 +7284,28 @@
         <v>34</v>
       </c>
       <c r="L1" t="s">
-        <v>169</v>
+        <v>134</v>
       </c>
       <c r="M1" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
       <c r="N1" t="s">
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="O1" t="s">
         <v>30</v>
       </c>
       <c r="P1" t="s">
-        <v>165</v>
+        <v>130</v>
       </c>
       <c r="Q1" t="s">
-        <v>167</v>
+        <v>132</v>
       </c>
       <c r="R1" t="s">
-        <v>173</v>
+        <v>138</v>
       </c>
       <c r="S1" t="s">
-        <v>168</v>
+        <v>133</v>
       </c>
       <c r="T1" t="s">
         <v>17</v>
@@ -7440,7 +7320,7 @@
         <v>18</v>
       </c>
       <c r="X1" t="s">
-        <v>163</v>
+        <v>128</v>
       </c>
       <c r="Y1" t="s">
         <v>22</v>
@@ -7448,7 +7328,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B2" t="n">
         <v>-0.1866419792452051</v>
@@ -7525,7 +7405,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>181</v>
+        <v>146</v>
       </c>
       <c r="B3" t="n">
         <v>-0.03579849024427175</v>
@@ -7602,7 +7482,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>182</v>
+        <v>102</v>
       </c>
       <c r="B4" t="n">
         <v>0.29355771297778177</v>
@@ -7679,7 +7559,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>183</v>
+        <v>106</v>
       </c>
       <c r="B5" t="n">
         <v>0.2825721119142708</v>
@@ -7756,7 +7636,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>184</v>
+        <v>147</v>
       </c>
       <c r="B6" t="n">
         <v>0.3593014672784915</v>
@@ -7833,7 +7713,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>185</v>
+        <v>89</v>
       </c>
       <c r="B7" t="n">
         <v>-0.30547439701197554</v>
@@ -7910,7 +7790,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B8" t="n">
         <v>0.0759973843657458</v>
@@ -7987,7 +7867,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>124</v>
+        <v>76</v>
       </c>
       <c r="B9" t="n">
         <v>0.21391479508700062</v>
@@ -8064,7 +7944,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>186</v>
+        <v>72</v>
       </c>
       <c r="B10" t="n">
         <v>0.3549496492454697</v>
@@ -8141,7 +8021,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>187</v>
+        <v>148</v>
       </c>
       <c r="B11" t="n">
         <v>0.21515876526077937</v>
@@ -8218,7 +8098,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>188</v>
+        <v>149</v>
       </c>
       <c r="B12" t="n">
         <v>-0.2620802392445565</v>
@@ -8295,7 +8175,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>189</v>
+        <v>150</v>
       </c>
       <c r="B13" t="n">
         <v>0.0663687528660774</v>
@@ -8372,7 +8252,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>190</v>
+        <v>151</v>
       </c>
       <c r="B14" t="n">
         <v>-0.28976488779395293</v>
@@ -8449,7 +8329,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>191</v>
+        <v>90</v>
       </c>
       <c r="B15" t="n">
         <v>-0.13836970234172996</v>
@@ -8526,7 +8406,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>192</v>
+        <v>152</v>
       </c>
       <c r="B16" t="n">
         <v>-0.31018462765351973</v>
@@ -8603,7 +8483,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>193</v>
+        <v>153</v>
       </c>
       <c r="B17" t="n">
         <v>0.3157421186918964</v>
@@ -8706,19 +8586,19 @@
         <v>20</v>
       </c>
       <c r="F1" t="s">
-        <v>163</v>
+        <v>128</v>
       </c>
       <c r="G1" t="s">
         <v>22</v>
       </c>
       <c r="H1" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="I1" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
       <c r="J1" t="s">
-        <v>167</v>
+        <v>132</v>
       </c>
       <c r="K1" t="s">
         <v>38</v>
@@ -8730,10 +8610,10 @@
         <v>40</v>
       </c>
       <c r="N1" t="s">
-        <v>165</v>
+        <v>130</v>
       </c>
       <c r="O1" t="s">
-        <v>173</v>
+        <v>138</v>
       </c>
       <c r="P1" t="s">
         <v>34</v>
@@ -8742,7 +8622,7 @@
         <v>35</v>
       </c>
       <c r="R1" t="s">
-        <v>171</v>
+        <v>136</v>
       </c>
       <c r="S1" t="s">
         <v>33</v>
@@ -8751,13 +8631,13 @@
         <v>32</v>
       </c>
       <c r="U1" t="s">
-        <v>168</v>
+        <v>133</v>
       </c>
       <c r="V1" t="s">
-        <v>169</v>
+        <v>134</v>
       </c>
       <c r="W1" t="s">
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="X1" t="s">
         <v>30</v>
@@ -8839,7 +8719,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>174</v>
+        <v>139</v>
       </c>
       <c r="B3" t="n">
         <v>-0.0697315990732736</v>
@@ -8913,7 +8793,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>175</v>
+        <v>140</v>
       </c>
       <c r="B4" t="n">
         <v>-0.2399476985840332</v>
@@ -8987,7 +8867,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>176</v>
+        <v>141</v>
       </c>
       <c r="B5" t="n">
         <v>-0.2013942565094806</v>
@@ -9061,7 +8941,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>177</v>
+        <v>142</v>
       </c>
       <c r="B6" t="n">
         <v>-0.3278458380490366</v>
@@ -9135,7 +9015,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>178</v>
+        <v>143</v>
       </c>
       <c r="B7" t="n">
         <v>-0.28676047626495915</v>
@@ -9209,7 +9089,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>179</v>
+        <v>144</v>
       </c>
       <c r="B8" t="n">
         <v>-0.013579209966020231</v>
@@ -9331,13 +9211,13 @@
         <v>41</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
         <v>41</v>
       </c>
       <c r="G2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3">
@@ -9354,13 +9234,13 @@
         <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F3" t="s">
         <v>41</v>
       </c>
       <c r="G3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4">
@@ -9377,13 +9257,13 @@
         <v>41</v>
       </c>
       <c r="E4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F4" t="s">
         <v>41</v>
       </c>
       <c r="G4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5">
@@ -9400,13 +9280,13 @@
         <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F5" t="s">
         <v>41</v>
       </c>
       <c r="G5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6">
@@ -9423,13 +9303,13 @@
         <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F6" t="s">
         <v>41</v>
       </c>
       <c r="G6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7">
@@ -9446,13 +9326,13 @@
         <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F7" t="s">
         <v>41</v>
       </c>
       <c r="G7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8">
@@ -9469,13 +9349,13 @@
         <v>41</v>
       </c>
       <c r="E8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F8" t="s">
         <v>41</v>
       </c>
       <c r="G8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9">
@@ -9492,13 +9372,13 @@
         <v>41</v>
       </c>
       <c r="E9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F9" t="s">
         <v>41</v>
       </c>
       <c r="G9" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10">
@@ -9515,13 +9395,13 @@
         <v>41</v>
       </c>
       <c r="E10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F10" t="s">
         <v>41</v>
       </c>
       <c r="G10" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11">
@@ -9538,13 +9418,13 @@
         <v>41</v>
       </c>
       <c r="E11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F11" t="s">
         <v>41</v>
       </c>
       <c r="G11" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12">
@@ -9561,13 +9441,13 @@
         <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F12" t="s">
         <v>41</v>
       </c>
       <c r="G12" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13">
@@ -9584,13 +9464,13 @@
         <v>41</v>
       </c>
       <c r="E13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F13" t="s">
         <v>41</v>
       </c>
       <c r="G13" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14">
@@ -9607,13 +9487,13 @@
         <v>41</v>
       </c>
       <c r="E14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F14" t="s">
         <v>41</v>
       </c>
       <c r="G14" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15">
@@ -9630,13 +9510,13 @@
         <v>41</v>
       </c>
       <c r="E15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F15" t="s">
         <v>41</v>
       </c>
       <c r="G15" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16">
@@ -9653,13 +9533,13 @@
         <v>42</v>
       </c>
       <c r="E16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F16" t="s">
         <v>41</v>
       </c>
       <c r="G16" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17">
@@ -9670,19 +9550,19 @@
         <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D17" t="s">
         <v>41</v>
       </c>
       <c r="E17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F17" t="s">
         <v>41</v>
       </c>
       <c r="G17" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18">
@@ -9693,19 +9573,19 @@
         <v>42</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D18" t="s">
         <v>42</v>
       </c>
       <c r="E18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F18" t="s">
         <v>42</v>
       </c>
       <c r="G18" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19">
@@ -9716,19 +9596,19 @@
         <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D19" t="s">
         <v>41</v>
       </c>
       <c r="E19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F19" t="s">
         <v>41</v>
       </c>
       <c r="G19" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20">
@@ -9739,19 +9619,19 @@
         <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D20" t="s">
         <v>41</v>
       </c>
       <c r="E20" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F20" t="s">
         <v>41</v>
       </c>
       <c r="G20" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21">
@@ -9762,19 +9642,19 @@
         <v>42</v>
       </c>
       <c r="C21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D21" t="s">
         <v>42</v>
       </c>
       <c r="E21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F21" t="s">
         <v>42</v>
       </c>
       <c r="G21" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22">
@@ -9785,19 +9665,19 @@
         <v>42</v>
       </c>
       <c r="C22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D22" t="s">
         <v>41</v>
       </c>
       <c r="E22" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="F22" t="s">
         <v>41</v>
       </c>
       <c r="G22" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23">
@@ -9808,19 +9688,19 @@
         <v>42</v>
       </c>
       <c r="C23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D23" t="s">
         <v>41</v>
       </c>
       <c r="E23" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F23" t="s">
         <v>41</v>
       </c>
       <c r="G23" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24">
@@ -9837,13 +9717,13 @@
         <v>41</v>
       </c>
       <c r="E24" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F24" t="s">
         <v>41</v>
       </c>
       <c r="G24" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25">
@@ -9860,13 +9740,13 @@
         <v>41</v>
       </c>
       <c r="E25" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F25" t="s">
         <v>41</v>
       </c>
       <c r="G25" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -9885,34 +9765,34 @@
     <row r="1">
       <c r="A1"/>
       <c r="B1" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="C1" t="s">
-        <v>168</v>
+        <v>133</v>
       </c>
       <c r="D1" t="s">
-        <v>165</v>
+        <v>130</v>
       </c>
       <c r="E1" t="s">
-        <v>173</v>
+        <v>138</v>
       </c>
       <c r="F1" t="s">
-        <v>169</v>
+        <v>134</v>
       </c>
       <c r="G1" t="s">
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="H1" t="s">
         <v>30</v>
       </c>
       <c r="I1" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
       <c r="J1" t="s">
-        <v>167</v>
+        <v>132</v>
       </c>
       <c r="K1" t="s">
-        <v>171</v>
+        <v>136</v>
       </c>
       <c r="L1" t="s">
         <v>33</v>
@@ -9948,7 +9828,7 @@
         <v>18</v>
       </c>
       <c r="W1" t="s">
-        <v>163</v>
+        <v>128</v>
       </c>
       <c r="X1" t="s">
         <v>22</v>
@@ -9956,7 +9836,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" t="n">
         <v>-0.33294844586843564</v>
@@ -10030,7 +9910,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" t="n">
         <v>-0.3150756881508476</v>
@@ -10104,7 +9984,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B4" t="n">
         <v>0.6081766146907289</v>
@@ -10178,7 +10058,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B5" t="n">
         <v>0.1592668711669817</v>
@@ -10252,7 +10132,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>139</v>
+        <v>85</v>
       </c>
       <c r="B6" t="n">
         <v>0.6863219002847833</v>
@@ -10326,7 +10206,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7" t="n">
         <v>-0.47885881159378463</v>
@@ -10400,7 +10280,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B8" t="n">
         <v>0.22130442238291967</v>
@@ -10474,7 +10354,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B9" t="n">
         <v>0.4855848418813363</v>
@@ -10548,7 +10428,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>180</v>
+        <v>145</v>
       </c>
       <c r="B10" t="n">
         <v>-0.410600418467738</v>
@@ -10645,7 +10525,7 @@
         <v>38</v>
       </c>
       <c r="E1" t="s">
-        <v>171</v>
+        <v>136</v>
       </c>
       <c r="F1" t="s">
         <v>33</v>
@@ -10660,28 +10540,28 @@
         <v>32</v>
       </c>
       <c r="J1" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="K1" t="s">
-        <v>167</v>
+        <v>132</v>
       </c>
       <c r="L1" t="s">
-        <v>168</v>
+        <v>133</v>
       </c>
       <c r="M1" t="s">
-        <v>165</v>
+        <v>130</v>
       </c>
       <c r="N1" t="s">
-        <v>173</v>
+        <v>138</v>
       </c>
       <c r="O1" t="s">
-        <v>169</v>
+        <v>134</v>
       </c>
       <c r="P1" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
       <c r="Q1" t="s">
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="R1" t="s">
         <v>30</v>
@@ -10690,7 +10570,7 @@
         <v>17</v>
       </c>
       <c r="T1" t="s">
-        <v>163</v>
+        <v>128</v>
       </c>
       <c r="U1" t="s">
         <v>22</v>
@@ -10707,7 +10587,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B2" t="n">
         <v>-0.19155342146511628</v>
@@ -10781,7 +10661,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>181</v>
+        <v>146</v>
       </c>
       <c r="B3" t="n">
         <v>-0.06333574273638634</v>
@@ -10855,7 +10735,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>182</v>
+        <v>102</v>
       </c>
       <c r="B4" t="n">
         <v>0.3245900033458808</v>
@@ -10929,7 +10809,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>183</v>
+        <v>106</v>
       </c>
       <c r="B5" t="n">
         <v>0.314358823333973</v>
@@ -11003,7 +10883,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>184</v>
+        <v>147</v>
       </c>
       <c r="B6" t="n">
         <v>0.3840274030142885</v>
@@ -11077,7 +10957,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>185</v>
+        <v>89</v>
       </c>
       <c r="B7" t="n">
         <v>-0.3333663140794375</v>
@@ -11151,7 +11031,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B8" t="n">
         <v>0.12048291408660976</v>
@@ -11225,7 +11105,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>124</v>
+        <v>76</v>
       </c>
       <c r="B9" t="n">
         <v>0.22388279219487994</v>
@@ -11299,7 +11179,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>186</v>
+        <v>72</v>
       </c>
       <c r="B10" t="n">
         <v>0.383285557547709</v>
@@ -11373,7 +11253,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>187</v>
+        <v>148</v>
       </c>
       <c r="B11" t="n">
         <v>0.2136571691401528</v>
@@ -11447,7 +11327,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>188</v>
+        <v>149</v>
       </c>
       <c r="B12" t="n">
         <v>-0.28503876821710195</v>
@@ -11521,7 +11401,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>189</v>
+        <v>150</v>
       </c>
       <c r="B13" t="n">
         <v>0.1089068701709208</v>
@@ -11595,7 +11475,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>190</v>
+        <v>151</v>
       </c>
       <c r="B14" t="n">
         <v>-0.28442472087542625</v>
@@ -11669,7 +11549,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>191</v>
+        <v>90</v>
       </c>
       <c r="B15" t="n">
         <v>-0.16935308432970242</v>
@@ -11743,7 +11623,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>192</v>
+        <v>152</v>
       </c>
       <c r="B16" t="n">
         <v>-0.34073520727588336</v>
@@ -11817,7 +11697,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>193</v>
+        <v>153</v>
       </c>
       <c r="B17" t="n">
         <v>0.3364795773624124</v>
@@ -11939,13 +11819,13 @@
         <v>41</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
         <v>41</v>
       </c>
       <c r="G2" t="s">
-        <v>102</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3">
@@ -11962,13 +11842,13 @@
         <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="F3" t="s">
         <v>41</v>
       </c>
       <c r="G3" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4">
@@ -11985,13 +11865,13 @@
         <v>41</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F4" t="s">
         <v>41</v>
       </c>
       <c r="G4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5">
@@ -12008,13 +11888,13 @@
         <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F5" t="s">
         <v>41</v>
       </c>
       <c r="G5" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6">
@@ -12025,19 +11905,19 @@
         <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>90</v>
+        <v>44</v>
       </c>
       <c r="D6" t="s">
         <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F6" t="s">
         <v>41</v>
       </c>
       <c r="G6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7">
@@ -12054,13 +11934,13 @@
         <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F7" t="s">
         <v>41</v>
       </c>
       <c r="G7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8">
@@ -12077,13 +11957,13 @@
         <v>41</v>
       </c>
       <c r="E8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F8" t="s">
         <v>41</v>
       </c>
       <c r="G8" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9">
@@ -12100,13 +11980,13 @@
         <v>41</v>
       </c>
       <c r="E9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F9" t="s">
         <v>41</v>
       </c>
       <c r="G9" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10">
@@ -12123,13 +12003,13 @@
         <v>41</v>
       </c>
       <c r="E10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F10" t="s">
         <v>41</v>
       </c>
       <c r="G10" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11">
@@ -12146,13 +12026,13 @@
         <v>41</v>
       </c>
       <c r="E11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F11" t="s">
         <v>41</v>
       </c>
       <c r="G11" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12">
@@ -12169,13 +12049,13 @@
         <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F12" t="s">
         <v>41</v>
       </c>
       <c r="G12" t="s">
-        <v>104</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13">
@@ -12192,13 +12072,13 @@
         <v>41</v>
       </c>
       <c r="E13" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="F13" t="s">
         <v>41</v>
       </c>
       <c r="G13" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14">
@@ -12215,13 +12095,13 @@
         <v>41</v>
       </c>
       <c r="E14" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="F14" t="s">
         <v>41</v>
       </c>
       <c r="G14" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15">
@@ -12238,13 +12118,13 @@
         <v>41</v>
       </c>
       <c r="E15" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="F15" t="s">
         <v>41</v>
       </c>
       <c r="G15" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16">
@@ -12255,19 +12135,19 @@
         <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D16" t="s">
         <v>41</v>
       </c>
       <c r="E16" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="F16" t="s">
         <v>41</v>
       </c>
       <c r="G16" t="s">
-        <v>108</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17">
@@ -12278,19 +12158,19 @@
         <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D17" t="s">
         <v>41</v>
       </c>
       <c r="E17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F17" t="s">
         <v>41</v>
       </c>
       <c r="G17" t="s">
-        <v>109</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18">
@@ -12301,19 +12181,19 @@
         <v>42</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D18" t="s">
         <v>42</v>
       </c>
       <c r="E18" t="s">
-        <v>97</v>
+        <v>63</v>
       </c>
       <c r="F18" t="s">
         <v>41</v>
       </c>
       <c r="G18" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19">
@@ -12324,19 +12204,19 @@
         <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D19" t="s">
         <v>41</v>
       </c>
       <c r="E19" t="s">
-        <v>98</v>
+        <v>62</v>
       </c>
       <c r="F19" t="s">
         <v>41</v>
       </c>
       <c r="G19" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20">
@@ -12347,19 +12227,19 @@
         <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D20" t="s">
         <v>41</v>
       </c>
       <c r="E20" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="F20" t="s">
         <v>41</v>
       </c>
       <c r="G20" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21">
@@ -12376,13 +12256,13 @@
         <v>41</v>
       </c>
       <c r="E21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F21" t="s">
         <v>41</v>
       </c>
       <c r="G21" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22">
@@ -12399,13 +12279,13 @@
         <v>41</v>
       </c>
       <c r="E22" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F22" t="s">
         <v>41</v>
       </c>
       <c r="G22" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23">
@@ -12416,19 +12296,19 @@
         <v>42</v>
       </c>
       <c r="C23" t="s">
-        <v>92</v>
+        <v>51</v>
       </c>
       <c r="D23" t="s">
         <v>41</v>
       </c>
       <c r="E23" t="s">
-        <v>100</v>
+        <v>58</v>
       </c>
       <c r="F23" t="s">
         <v>41</v>
       </c>
       <c r="G23" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24">
@@ -12439,19 +12319,19 @@
         <v>42</v>
       </c>
       <c r="C24" t="s">
-        <v>93</v>
+        <v>51</v>
       </c>
       <c r="D24" t="s">
         <v>41</v>
       </c>
       <c r="E24" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="F24" t="s">
         <v>41</v>
       </c>
       <c r="G24" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -12504,13 +12384,13 @@
         <v>41</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
         <v>41</v>
       </c>
       <c r="G2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3">
@@ -12527,13 +12407,13 @@
         <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F3" t="s">
         <v>41</v>
       </c>
       <c r="G3" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4">
@@ -12550,13 +12430,13 @@
         <v>41</v>
       </c>
       <c r="E4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F4" t="s">
         <v>41</v>
       </c>
       <c r="G4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5">
@@ -12573,13 +12453,13 @@
         <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F5" t="s">
         <v>41</v>
       </c>
       <c r="G5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6">
@@ -12590,19 +12470,19 @@
         <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>90</v>
+        <v>44</v>
       </c>
       <c r="D6" t="s">
         <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F6" t="s">
         <v>41</v>
       </c>
       <c r="G6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7">
@@ -12613,19 +12493,19 @@
         <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>114</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s">
         <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F7" t="s">
         <v>41</v>
       </c>
       <c r="G7" t="s">
-        <v>121</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8">
@@ -12642,13 +12522,13 @@
         <v>41</v>
       </c>
       <c r="E8" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="F8" t="s">
         <v>41</v>
       </c>
       <c r="G8" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9">
@@ -12659,19 +12539,19 @@
         <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9" t="s">
         <v>42</v>
       </c>
       <c r="E9" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="F9" t="s">
         <v>42</v>
       </c>
       <c r="G9" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10">
@@ -12682,19 +12562,19 @@
         <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D10" t="s">
         <v>42</v>
       </c>
       <c r="E10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F10" t="s">
         <v>41</v>
       </c>
       <c r="G10" t="s">
-        <v>124</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11">
@@ -12705,19 +12585,19 @@
         <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D11" t="s">
         <v>42</v>
       </c>
       <c r="E11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F11" t="s">
         <v>42</v>
       </c>
       <c r="G11" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12">
@@ -12728,19 +12608,19 @@
         <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D12" t="s">
         <v>42</v>
       </c>
       <c r="E12" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="F12" t="s">
         <v>42</v>
       </c>
       <c r="G12" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13">
@@ -12751,19 +12631,19 @@
         <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D13" t="s">
         <v>42</v>
       </c>
       <c r="E13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F13" t="s">
         <v>42</v>
       </c>
       <c r="G13" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14">
@@ -12780,13 +12660,13 @@
         <v>41</v>
       </c>
       <c r="E14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F14" t="s">
         <v>41</v>
       </c>
       <c r="G14" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15">
@@ -12803,13 +12683,13 @@
         <v>41</v>
       </c>
       <c r="E15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F15" t="s">
         <v>41</v>
       </c>
       <c r="G15" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16">
@@ -12826,13 +12706,13 @@
         <v>41</v>
       </c>
       <c r="E16" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F16" t="s">
         <v>41</v>
       </c>
       <c r="G16" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17">
@@ -12849,13 +12729,13 @@
         <v>41</v>
       </c>
       <c r="E17" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="F17" t="s">
         <v>41</v>
       </c>
       <c r="G17" t="s">
-        <v>129</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18">
@@ -12866,19 +12746,19 @@
         <v>42</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D18" t="s">
         <v>41</v>
       </c>
       <c r="E18" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="F18" t="s">
         <v>41</v>
       </c>
       <c r="G18" t="s">
-        <v>130</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19">
@@ -12895,13 +12775,13 @@
         <v>41</v>
       </c>
       <c r="E19" t="s">
-        <v>118</v>
+        <v>86</v>
       </c>
       <c r="F19" t="s">
         <v>41</v>
       </c>
       <c r="G19" t="s">
-        <v>131</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20">
@@ -12918,13 +12798,13 @@
         <v>41</v>
       </c>
       <c r="E20" t="s">
-        <v>119</v>
+        <v>59</v>
       </c>
       <c r="F20" t="s">
         <v>41</v>
       </c>
       <c r="G20" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21">
@@ -12935,19 +12815,19 @@
         <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>115</v>
+        <v>45</v>
       </c>
       <c r="D21" t="s">
         <v>41</v>
       </c>
       <c r="E21" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="F21" t="s">
         <v>41</v>
       </c>
       <c r="G21" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22">
@@ -12964,13 +12844,13 @@
         <v>41</v>
       </c>
       <c r="E22" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F22" t="s">
         <v>41</v>
       </c>
       <c r="G22" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23">
@@ -12987,13 +12867,13 @@
         <v>41</v>
       </c>
       <c r="E23" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F23" t="s">
         <v>41</v>
       </c>
       <c r="G23" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24">
@@ -13010,13 +12890,13 @@
         <v>41</v>
       </c>
       <c r="E24" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F24" t="s">
         <v>41</v>
       </c>
       <c r="G24" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -13069,13 +12949,13 @@
         <v>41</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
         <v>41</v>
       </c>
       <c r="G2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3">
@@ -13092,13 +12972,13 @@
         <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F3" t="s">
         <v>41</v>
       </c>
       <c r="G3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4">
@@ -13115,13 +12995,13 @@
         <v>41</v>
       </c>
       <c r="E4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F4" t="s">
         <v>41</v>
       </c>
       <c r="G4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5">
@@ -13138,13 +13018,13 @@
         <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F5" t="s">
         <v>41</v>
       </c>
       <c r="G5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6">
@@ -13161,13 +13041,13 @@
         <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="F6" t="s">
         <v>41</v>
       </c>
       <c r="G6" t="s">
-        <v>143</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7">
@@ -13184,13 +13064,13 @@
         <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>137</v>
+        <v>53</v>
       </c>
       <c r="F7" t="s">
         <v>41</v>
       </c>
       <c r="G7" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8">
@@ -13207,13 +13087,13 @@
         <v>41</v>
       </c>
       <c r="E8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F8" t="s">
         <v>41</v>
       </c>
       <c r="G8" t="s">
-        <v>144</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9">
@@ -13230,13 +13110,13 @@
         <v>41</v>
       </c>
       <c r="E9" t="s">
-        <v>138</v>
+        <v>59</v>
       </c>
       <c r="F9" t="s">
         <v>41</v>
       </c>
       <c r="G9" t="s">
-        <v>145</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10">
@@ -13253,13 +13133,13 @@
         <v>41</v>
       </c>
       <c r="E10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F10" t="s">
         <v>41</v>
       </c>
       <c r="G10" t="s">
-        <v>146</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11">
@@ -13276,13 +13156,13 @@
         <v>41</v>
       </c>
       <c r="E11" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="F11" t="s">
         <v>41</v>
       </c>
       <c r="G11" t="s">
-        <v>147</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12">
@@ -13299,13 +13179,13 @@
         <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>139</v>
+        <v>85</v>
       </c>
       <c r="F12" t="s">
         <v>41</v>
       </c>
       <c r="G12" t="s">
-        <v>148</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13">
@@ -13322,13 +13202,13 @@
         <v>41</v>
       </c>
       <c r="E13" t="s">
-        <v>140</v>
+        <v>85</v>
       </c>
       <c r="F13" t="s">
         <v>41</v>
       </c>
       <c r="G13" t="s">
-        <v>149</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14">
@@ -13345,13 +13225,13 @@
         <v>41</v>
       </c>
       <c r="E14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F14" t="s">
         <v>41</v>
       </c>
       <c r="G14" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15">
@@ -13368,13 +13248,13 @@
         <v>41</v>
       </c>
       <c r="E15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F15" t="s">
         <v>41</v>
       </c>
       <c r="G15" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16">
@@ -13391,13 +13271,13 @@
         <v>41</v>
       </c>
       <c r="E16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F16" t="s">
         <v>41</v>
       </c>
       <c r="G16" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17">
@@ -13408,19 +13288,19 @@
         <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>111</v>
       </c>
       <c r="D17" t="s">
         <v>41</v>
       </c>
       <c r="E17" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F17" t="s">
         <v>41</v>
       </c>
       <c r="G17" t="s">
-        <v>150</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18">
@@ -13437,13 +13317,13 @@
         <v>41</v>
       </c>
       <c r="E18" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F18" t="s">
         <v>41</v>
       </c>
       <c r="G18" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19">
@@ -13460,13 +13340,13 @@
         <v>41</v>
       </c>
       <c r="E19" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F19" t="s">
         <v>41</v>
       </c>
       <c r="G19" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20">
@@ -13477,19 +13357,19 @@
         <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>134</v>
+        <v>112</v>
       </c>
       <c r="D20" t="s">
         <v>42</v>
       </c>
       <c r="E20" t="s">
-        <v>141</v>
+        <v>115</v>
       </c>
       <c r="F20" t="s">
         <v>42</v>
       </c>
       <c r="G20" t="s">
-        <v>151</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21">
@@ -13500,19 +13380,19 @@
         <v>42</v>
       </c>
       <c r="C21" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="D21" t="s">
         <v>42</v>
       </c>
       <c r="E21" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="F21" t="s">
         <v>41</v>
       </c>
       <c r="G21" t="s">
-        <v>152</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22">
@@ -13523,19 +13403,19 @@
         <v>42</v>
       </c>
       <c r="C22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D22" t="s">
         <v>42</v>
       </c>
       <c r="E22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F22" t="s">
         <v>42</v>
       </c>
       <c r="G22" t="s">
-        <v>153</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23">
@@ -13546,19 +13426,19 @@
         <v>42</v>
       </c>
       <c r="C23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D23" t="s">
         <v>41</v>
       </c>
       <c r="E23" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F23" t="s">
         <v>41</v>
       </c>
       <c r="G23" t="s">
-        <v>124</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24">
@@ -13569,19 +13449,19 @@
         <v>42</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D24" t="s">
         <v>42</v>
       </c>
       <c r="E24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F24" t="s">
         <v>41</v>
       </c>
       <c r="G24" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25">
@@ -13592,19 +13472,19 @@
         <v>42</v>
       </c>
       <c r="C25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D25" t="s">
         <v>41</v>
       </c>
       <c r="E25" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F25" t="s">
         <v>41</v>
       </c>
       <c r="G25" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -13657,13 +13537,13 @@
         <v>41</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
         <v>41</v>
       </c>
       <c r="G2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3">
@@ -13680,13 +13560,13 @@
         <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F3" t="s">
         <v>41</v>
       </c>
       <c r="G3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4">
@@ -13703,13 +13583,13 @@
         <v>41</v>
       </c>
       <c r="E4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F4" t="s">
         <v>41</v>
       </c>
       <c r="G4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5">
@@ -13726,13 +13606,13 @@
         <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F5" t="s">
         <v>41</v>
       </c>
       <c r="G5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6">
@@ -13749,13 +13629,13 @@
         <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F6" t="s">
         <v>41</v>
       </c>
       <c r="G6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7">
@@ -13772,13 +13652,13 @@
         <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>137</v>
+        <v>53</v>
       </c>
       <c r="F7" t="s">
         <v>41</v>
       </c>
       <c r="G7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8">
@@ -13795,13 +13675,13 @@
         <v>41</v>
       </c>
       <c r="E8" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="F8" t="s">
         <v>41</v>
       </c>
       <c r="G8" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9">
@@ -13818,13 +13698,13 @@
         <v>41</v>
       </c>
       <c r="E9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F9" t="s">
         <v>41</v>
       </c>
       <c r="G9" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10">
@@ -13841,13 +13721,13 @@
         <v>41</v>
       </c>
       <c r="E10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F10" t="s">
         <v>41</v>
       </c>
       <c r="G10" t="s">
-        <v>104</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11">
@@ -13858,19 +13738,19 @@
         <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>154</v>
+        <v>51</v>
       </c>
       <c r="D11" t="s">
         <v>41</v>
       </c>
       <c r="E11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F11" t="s">
         <v>41</v>
       </c>
       <c r="G11" t="s">
-        <v>159</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12">
@@ -13887,13 +13767,13 @@
         <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F12" t="s">
         <v>41</v>
       </c>
       <c r="G12" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13">
@@ -13910,13 +13790,13 @@
         <v>41</v>
       </c>
       <c r="E13" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F13" t="s">
         <v>41</v>
       </c>
       <c r="G13" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14">
@@ -13933,13 +13813,13 @@
         <v>41</v>
       </c>
       <c r="E14" t="s">
-        <v>118</v>
+        <v>86</v>
       </c>
       <c r="F14" t="s">
         <v>41</v>
       </c>
       <c r="G14" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15">
@@ -13950,19 +13830,19 @@
         <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>155</v>
+        <v>124</v>
       </c>
       <c r="D15" t="s">
         <v>41</v>
       </c>
       <c r="E15" t="s">
-        <v>157</v>
+        <v>58</v>
       </c>
       <c r="F15" t="s">
         <v>41</v>
       </c>
       <c r="G15" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16">
@@ -13973,19 +13853,19 @@
         <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D16" t="s">
         <v>42</v>
       </c>
       <c r="E16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F16" t="s">
         <v>42</v>
       </c>
       <c r="G16" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17">
@@ -13996,19 +13876,19 @@
         <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D17" t="s">
         <v>41</v>
       </c>
       <c r="E17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F17" t="s">
         <v>41</v>
       </c>
       <c r="G17" t="s">
-        <v>124</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18">
@@ -14019,19 +13899,19 @@
         <v>42</v>
       </c>
       <c r="C18" t="s">
-        <v>156</v>
+        <v>125</v>
       </c>
       <c r="D18" t="s">
         <v>42</v>
       </c>
       <c r="E18" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F18" t="s">
         <v>41</v>
       </c>
       <c r="G18" t="s">
-        <v>160</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19">
@@ -14042,19 +13922,19 @@
         <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D19" t="s">
         <v>42</v>
       </c>
       <c r="E19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F19" t="s">
         <v>42</v>
       </c>
       <c r="G19" t="s">
-        <v>161</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20">
@@ -14065,19 +13945,19 @@
         <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D20" t="s">
         <v>41</v>
       </c>
       <c r="E20" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F20" t="s">
         <v>41</v>
       </c>
       <c r="G20" t="s">
-        <v>124</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21">
@@ -14088,19 +13968,19 @@
         <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="D21" t="s">
         <v>41</v>
       </c>
       <c r="E21" t="s">
-        <v>158</v>
+        <v>60</v>
       </c>
       <c r="F21" t="s">
         <v>41</v>
       </c>
       <c r="G21" t="s">
-        <v>162</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22">
@@ -14117,13 +13997,13 @@
         <v>41</v>
       </c>
       <c r="E22" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F22" t="s">
         <v>41</v>
       </c>
       <c r="G22" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23">
@@ -14140,13 +14020,13 @@
         <v>41</v>
       </c>
       <c r="E23" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F23" t="s">
         <v>41</v>
       </c>
       <c r="G23" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24">
@@ -14163,13 +14043,13 @@
         <v>41</v>
       </c>
       <c r="E24" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F24" t="s">
         <v>41</v>
       </c>
       <c r="G24" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -14200,37 +14080,37 @@
         <v>20</v>
       </c>
       <c r="F1" t="s">
-        <v>163</v>
+        <v>128</v>
       </c>
       <c r="G1" t="s">
         <v>22</v>
       </c>
       <c r="H1" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="I1" t="s">
-        <v>165</v>
+        <v>130</v>
       </c>
       <c r="J1" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
       <c r="K1" t="s">
-        <v>167</v>
+        <v>132</v>
       </c>
       <c r="L1" t="s">
-        <v>168</v>
+        <v>133</v>
       </c>
       <c r="M1" t="s">
-        <v>169</v>
+        <v>134</v>
       </c>
       <c r="N1" t="s">
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="O1" t="s">
         <v>30</v>
       </c>
       <c r="P1" t="s">
-        <v>171</v>
+        <v>136</v>
       </c>
       <c r="Q1" t="s">
         <v>32</v>
@@ -14245,10 +14125,10 @@
         <v>35</v>
       </c>
       <c r="U1" t="s">
-        <v>172</v>
+        <v>137</v>
       </c>
       <c r="V1" t="s">
-        <v>173</v>
+        <v>138</v>
       </c>
       <c r="W1" t="s">
         <v>38</v>
@@ -14339,7 +14219,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>174</v>
+        <v>139</v>
       </c>
       <c r="B3" t="n">
         <v>-0.06097494071173785</v>
@@ -14416,7 +14296,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>175</v>
+        <v>140</v>
       </c>
       <c r="B4" t="n">
         <v>-0.23863368139486743</v>
@@ -14493,7 +14373,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>176</v>
+        <v>141</v>
       </c>
       <c r="B5" t="n">
         <v>-0.21061885930711005</v>
@@ -14570,7 +14450,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>177</v>
+        <v>142</v>
       </c>
       <c r="B6" t="n">
         <v>-0.3567210368080936</v>
@@ -14647,7 +14527,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>178</v>
+        <v>143</v>
       </c>
       <c r="B7" t="n">
         <v>-0.31832493178443616</v>
@@ -14724,7 +14604,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>179</v>
+        <v>144</v>
       </c>
       <c r="B8" t="n">
         <v>0.012252040283909473</v>
@@ -14815,34 +14695,34 @@
     <row r="1">
       <c r="A1"/>
       <c r="B1" t="s">
-        <v>168</v>
+        <v>133</v>
       </c>
       <c r="C1" t="s">
-        <v>165</v>
+        <v>130</v>
       </c>
       <c r="D1" t="s">
-        <v>173</v>
+        <v>138</v>
       </c>
       <c r="E1" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
       <c r="F1" t="s">
-        <v>167</v>
+        <v>132</v>
       </c>
       <c r="G1" t="s">
-        <v>169</v>
+        <v>134</v>
       </c>
       <c r="H1" t="s">
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="I1" t="s">
         <v>30</v>
       </c>
       <c r="J1" t="s">
-        <v>172</v>
+        <v>137</v>
       </c>
       <c r="K1" t="s">
-        <v>171</v>
+        <v>136</v>
       </c>
       <c r="L1" t="s">
         <v>34</v>
@@ -14857,7 +14737,7 @@
         <v>32</v>
       </c>
       <c r="P1" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="Q1" t="s">
         <v>39</v>
@@ -14881,7 +14761,7 @@
         <v>18</v>
       </c>
       <c r="X1" t="s">
-        <v>163</v>
+        <v>128</v>
       </c>
       <c r="Y1" t="s">
         <v>22</v>
@@ -14889,7 +14769,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" t="n">
         <v>-0.38161553668335185</v>
@@ -14966,7 +14846,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" t="n">
         <v>-0.4327461528442115</v>
@@ -15043,7 +14923,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B4" t="n">
         <v>0.3368659213181972</v>
@@ -15120,7 +15000,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B5" t="n">
         <v>0.3181384133844036</v>
@@ -15197,7 +15077,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>139</v>
+        <v>85</v>
       </c>
       <c r="B6" t="n">
         <v>0.4699933982766882</v>
@@ -15274,7 +15154,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7" t="n">
         <v>-0.4202809104897496</v>
@@ -15351,7 +15231,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B8" t="n">
         <v>0.6080612963953639</v>
@@ -15428,7 +15308,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B9" t="n">
         <v>0.3954667370319464</v>
@@ -15505,7 +15385,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>180</v>
+        <v>145</v>
       </c>
       <c r="B10" t="n">
         <v>-0.15961565196446553</v>
@@ -15596,31 +15476,31 @@
     <row r="1">
       <c r="A1"/>
       <c r="B1" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
       <c r="C1" t="s">
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="D1" t="s">
         <v>30</v>
       </c>
       <c r="E1" t="s">
-        <v>167</v>
+        <v>132</v>
       </c>
       <c r="F1" t="s">
-        <v>165</v>
+        <v>130</v>
       </c>
       <c r="G1" t="s">
-        <v>173</v>
+        <v>138</v>
       </c>
       <c r="H1" t="s">
-        <v>168</v>
+        <v>133</v>
       </c>
       <c r="I1" t="s">
-        <v>169</v>
+        <v>134</v>
       </c>
       <c r="J1" t="s">
-        <v>172</v>
+        <v>137</v>
       </c>
       <c r="K1" t="s">
         <v>39</v>
@@ -15632,7 +15512,7 @@
         <v>38</v>
       </c>
       <c r="N1" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="O1" t="s">
         <v>34</v>
@@ -15641,7 +15521,7 @@
         <v>35</v>
       </c>
       <c r="Q1" t="s">
-        <v>171</v>
+        <v>136</v>
       </c>
       <c r="R1" t="s">
         <v>33</v>
@@ -15653,7 +15533,7 @@
         <v>17</v>
       </c>
       <c r="U1" t="s">
-        <v>163</v>
+        <v>128</v>
       </c>
       <c r="V1" t="s">
         <v>22</v>
@@ -15670,7 +15550,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B2" t="n">
         <v>-0.34815142472904104</v>
@@ -15747,7 +15627,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>181</v>
+        <v>146</v>
       </c>
       <c r="B3" t="n">
         <v>-0.34283405981181564</v>
@@ -15824,7 +15704,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>182</v>
+        <v>102</v>
       </c>
       <c r="B4" t="n">
         <v>0.25310467177208756</v>
@@ -15901,7 +15781,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>183</v>
+        <v>106</v>
       </c>
       <c r="B5" t="n">
         <v>0.5432784203652965</v>
@@ -15978,7 +15858,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>184</v>
+        <v>147</v>
       </c>
       <c r="B6" t="n">
         <v>0.3278024651302813</v>
@@ -16055,7 +15935,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>185</v>
+        <v>89</v>
       </c>
       <c r="B7" t="n">
         <v>-0.3494968962345341</v>
@@ -16132,7 +16012,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B8" t="n">
         <v>0.43585076602121614</v>
@@ -16209,7 +16089,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>124</v>
+        <v>76</v>
       </c>
       <c r="B9" t="n">
         <v>0.11987802065479551</v>
@@ -16286,7 +16166,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>186</v>
+        <v>72</v>
       </c>
       <c r="B10" t="n">
         <v>0.3577244292508561</v>
@@ -16363,7 +16243,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>187</v>
+        <v>148</v>
       </c>
       <c r="B11" t="n">
         <v>0.15419614028689632</v>
@@ -16440,7 +16320,7 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>188</v>
+        <v>149</v>
       </c>
       <c r="B12" t="n">
         <v>-0.14745611623069502</v>
@@ -16517,7 +16397,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>189</v>
+        <v>150</v>
       </c>
       <c r="B13" t="n">
         <v>0.400139074359011</v>
@@ -16594,7 +16474,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>190</v>
+        <v>151</v>
       </c>
       <c r="B14" t="n">
         <v>-0.014756793433096377</v>
@@ -16671,7 +16551,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>191</v>
+        <v>90</v>
       </c>
       <c r="B15" t="n">
         <v>-0.36570502131577326</v>
@@ -16748,7 +16628,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>192</v>
+        <v>152</v>
       </c>
       <c r="B16" t="n">
         <v>-0.2537751426739263</v>
@@ -16825,7 +16705,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>193</v>
+        <v>153</v>
       </c>
       <c r="B17" t="n">
         <v>0.4940267375409182</v>

</xml_diff>